<commit_message>
Actualizacion de proyecto,puliendo comparacion entre nexxim y BOM ademas de solucionar bugs anteriores
</commit_message>
<xml_diff>
--- a/23359-1D/23359-1D_top.xlsx
+++ b/23359-1D/23359-1D_top.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Temporal\Echevarria\23359-1D\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bconline-my.sharepoint.com/personal/cristian_echevarria_navicogroup_com/Documents/Documents/Proyectos_Python/PysimpleGUI/Proyectos/comparador/23359-1D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC8C07E-7775-4257-832F-A75FFAF08D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{FEC8C07E-7775-4257-832F-A75FFAF08D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5CBF048-AC66-4356-B357-2819C09B00D1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="1680" windowWidth="29040" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2630,6 +2630,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2897,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF602"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AF603"/>
+    <sheetView tabSelected="1" topLeftCell="A586" workbookViewId="0">
+      <selection activeCell="O616" sqref="O616"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>